<commit_message>
add copyright header to source files
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp_\ParaDIS\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1b30c35e24e816a/Документы/GitHub/ParaDIS/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284B29B3-E86C-47B0-B55A-85F868949C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{284B29B3-E86C-47B0-B55A-85F868949C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB46E581-21D7-40E0-AE90-75A742CB73A2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{652830A2-7AE8-4A1B-B7C6-41D38EC7B5AA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="58">
   <si>
     <t>RMSE</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>RT_train</t>
-  </si>
-  <si>
-    <t>н/д</t>
   </si>
   <si>
     <t>Run time, ms</t>
@@ -352,13 +349,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1030,19 +1027,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1077,30 +1068,6 @@
     <xf numFmtId="4" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1113,21 +1080,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1168,6 +1120,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1508,17 +1505,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E1" s="84" t="s">
+      <c r="E1" s="122" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="123"/>
+      <c r="G1" s="122" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="85"/>
-      <c r="G1" s="84" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="86"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="124"/>
     </row>
     <row r="2" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1574,20 +1571,20 @@
       <c r="F3" s="15">
         <v>0.05</v>
       </c>
-      <c r="G3" s="55">
+      <c r="G3" s="53">
         <v>1.95</v>
       </c>
-      <c r="H3" s="56">
+      <c r="H3" s="54">
         <v>0.28620800000000002</v>
       </c>
-      <c r="I3" s="56">
+      <c r="I3" s="54">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J3" s="66">
+      <c r="J3" s="64">
         <f t="shared" ref="J3:J8" si="0">G3*H3</f>
         <v>0.55810559999999998</v>
       </c>
-      <c r="K3" s="57">
+      <c r="K3" s="55">
         <v>0.05</v>
       </c>
     </row>
@@ -1619,11 +1616,11 @@
       <c r="I4" s="4">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J4" s="66">
+      <c r="J4" s="64">
         <f t="shared" si="0"/>
         <v>0.30051840000000002</v>
       </c>
-      <c r="K4" s="58">
+      <c r="K4" s="56">
         <v>0.47</v>
       </c>
     </row>
@@ -1655,11 +1652,11 @@
       <c r="I5" s="4">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J5" s="66">
+      <c r="J5" s="64">
         <f t="shared" si="0"/>
         <v>0.54093312000000005</v>
       </c>
-      <c r="K5" s="58">
+      <c r="K5" s="56">
         <v>0.09</v>
       </c>
     </row>
@@ -1679,7 +1676,7 @@
       <c r="E6" s="8">
         <v>0.75</v>
       </c>
-      <c r="F6" s="63">
+      <c r="F6" s="61">
         <v>0.19</v>
       </c>
       <c r="G6" s="9">
@@ -1691,11 +1688,11 @@
       <c r="I6" s="4">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J6" s="66">
+      <c r="J6" s="64">
         <f t="shared" si="0"/>
         <v>0.27475968000000001</v>
       </c>
-      <c r="K6" s="58">
+      <c r="K6" s="56">
         <v>0.37</v>
       </c>
     </row>
@@ -1715,7 +1712,7 @@
       <c r="E7" s="8">
         <v>0.43</v>
       </c>
-      <c r="F7" s="63">
+      <c r="F7" s="61">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G7" s="9">
@@ -1727,11 +1724,11 @@
       <c r="I7" s="4">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J7" s="66">
+      <c r="J7" s="64">
         <f t="shared" si="0"/>
         <v>0.44934656000000006</v>
       </c>
-      <c r="K7" s="58">
+      <c r="K7" s="56">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
@@ -1751,7 +1748,7 @@
       <c r="E8" s="8">
         <v>0.41</v>
       </c>
-      <c r="F8" s="64">
+      <c r="F8" s="62">
         <v>2</v>
       </c>
       <c r="G8" s="9">
@@ -1763,17 +1760,17 @@
       <c r="I8" s="4">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J8" s="66">
+      <c r="J8" s="64">
         <f t="shared" si="0"/>
         <v>0.40927743999999999</v>
       </c>
-      <c r="K8" s="58">
+      <c r="K8" s="56">
         <v>2.2599999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>13</v>
@@ -1787,18 +1784,18 @@
       <c r="E9" s="8">
         <v>0.03</v>
       </c>
-      <c r="F9" s="63">
+      <c r="F9" s="61">
         <v>0.8</v>
       </c>
-      <c r="G9" s="59"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="59"/>
     </row>
     <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>13</v>
@@ -1812,14 +1809,14 @@
       <c r="E10" s="8">
         <v>0.03</v>
       </c>
-      <c r="F10" s="63">
+      <c r="F10" s="61">
         <v>3.79</v>
       </c>
-      <c r="G10" s="59"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="61"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="59"/>
     </row>
     <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -1837,7 +1834,7 @@
       <c r="E11" s="9">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F11" s="62">
+      <c r="F11" s="60">
         <v>0.03</v>
       </c>
       <c r="G11" s="9">
@@ -1849,11 +1846,11 @@
       <c r="I11" s="4">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J11" s="66">
+      <c r="J11" s="64">
         <f t="shared" ref="J11:J16" si="1">G11*H11</f>
         <v>0.26044928000000001</v>
       </c>
-      <c r="K11" s="58">
+      <c r="K11" s="56">
         <v>0.03</v>
       </c>
     </row>
@@ -1873,7 +1870,7 @@
       <c r="E12" s="9">
         <v>0.59</v>
       </c>
-      <c r="F12" s="62">
+      <c r="F12" s="60">
         <v>2.58</v>
       </c>
       <c r="G12" s="9">
@@ -1885,11 +1882,11 @@
       <c r="I12" s="4">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J12" s="66">
+      <c r="J12" s="64">
         <f t="shared" si="1"/>
         <v>0.30051840000000002</v>
       </c>
-      <c r="K12" s="58">
+      <c r="K12" s="56">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -1909,7 +1906,7 @@
       <c r="E13" s="9">
         <v>0.21</v>
       </c>
-      <c r="F13" s="62">
+      <c r="F13" s="60">
         <v>0.12</v>
       </c>
       <c r="G13" s="9">
@@ -1921,11 +1918,11 @@
       <c r="I13" s="4">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J13" s="66">
+      <c r="J13" s="64">
         <f t="shared" si="1"/>
         <v>0.17744896000000002</v>
       </c>
-      <c r="K13" s="58">
+      <c r="K13" s="56">
         <v>0.11</v>
       </c>
     </row>
@@ -1945,7 +1942,7 @@
       <c r="E14" s="9">
         <v>0.08</v>
       </c>
-      <c r="F14" s="62">
+      <c r="F14" s="60">
         <v>1.1599999999999999</v>
       </c>
       <c r="G14" s="9">
@@ -1957,11 +1954,11 @@
       <c r="I14" s="4">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J14" s="66">
+      <c r="J14" s="64">
         <f t="shared" si="1"/>
         <v>0.14596608</v>
       </c>
-      <c r="K14" s="58">
+      <c r="K14" s="56">
         <v>0.32</v>
       </c>
     </row>
@@ -1981,7 +1978,7 @@
       <c r="E15" s="9">
         <v>0.1</v>
       </c>
-      <c r="F15" s="62">
+      <c r="F15" s="60">
         <v>0.02</v>
       </c>
       <c r="G15" s="9">
@@ -1993,11 +1990,11 @@
       <c r="I15" s="4">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J15" s="66">
+      <c r="J15" s="64">
         <f t="shared" si="1"/>
         <v>0.10017280000000001</v>
       </c>
-      <c r="K15" s="58">
+      <c r="K15" s="56">
         <v>0.02</v>
       </c>
     </row>
@@ -2017,7 +2014,7 @@
       <c r="E16" s="9">
         <v>0.41</v>
       </c>
-      <c r="F16" s="62">
+      <c r="F16" s="60">
         <v>2</v>
       </c>
       <c r="G16" s="9">
@@ -2029,17 +2026,17 @@
       <c r="I16" s="4">
         <v>0.68062900000000004</v>
       </c>
-      <c r="J16" s="66">
+      <c r="J16" s="64">
         <f t="shared" si="1"/>
         <v>0.40927743999999999</v>
       </c>
-      <c r="K16" s="58">
+      <c r="K16" s="56">
         <v>1.98</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>13</v>
@@ -2053,18 +2050,18 @@
       <c r="E17" s="9">
         <v>0.02</v>
       </c>
-      <c r="F17" s="62">
+      <c r="F17" s="60">
         <v>11.9</v>
       </c>
-      <c r="G17" s="59"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="61"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
     </row>
     <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>13</v>
@@ -2078,14 +2075,14 @@
       <c r="E18" s="9">
         <v>0.02</v>
       </c>
-      <c r="F18" s="63">
+      <c r="F18" s="61">
         <v>10.88</v>
       </c>
-      <c r="G18" s="59"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="61"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="59"/>
     </row>
     <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -2103,7 +2100,7 @@
       <c r="E19" s="9">
         <v>14.82</v>
       </c>
-      <c r="F19" s="62">
+      <c r="F19" s="60">
         <v>0.49</v>
       </c>
       <c r="G19" s="9">
@@ -2115,11 +2112,11 @@
       <c r="I19" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J19" s="66">
+      <c r="J19" s="64">
         <f t="shared" ref="J19:J24" si="2">G19*H19</f>
         <v>0.88515339000000004</v>
       </c>
-      <c r="K19" s="58">
+      <c r="K19" s="56">
         <v>0.5</v>
       </c>
     </row>
@@ -2139,7 +2136,7 @@
       <c r="E20" s="9">
         <v>1.18</v>
       </c>
-      <c r="F20" s="62">
+      <c r="F20" s="60">
         <v>1.23</v>
       </c>
       <c r="G20" s="9">
@@ -2151,11 +2148,11 @@
       <c r="I20" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J20" s="66">
+      <c r="J20" s="64">
         <f t="shared" si="2"/>
         <v>0.12736020000000001</v>
       </c>
-      <c r="K20" s="58">
+      <c r="K20" s="56">
         <v>1.25</v>
       </c>
     </row>
@@ -2175,7 +2172,7 @@
       <c r="E21" s="9">
         <v>10.029999999999999</v>
       </c>
-      <c r="F21" s="62">
+      <c r="F21" s="60">
         <v>0.09</v>
       </c>
       <c r="G21" s="9">
@@ -2187,11 +2184,11 @@
       <c r="I21" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J21" s="66">
+      <c r="J21" s="64">
         <f t="shared" si="2"/>
         <v>7.0048110000000011E-2</v>
       </c>
-      <c r="K21" s="58">
+      <c r="K21" s="56">
         <v>0.02</v>
       </c>
     </row>
@@ -2211,7 +2208,7 @@
       <c r="E22" s="9">
         <v>10.09</v>
       </c>
-      <c r="F22" s="62">
+      <c r="F22" s="60">
         <v>0.2</v>
       </c>
       <c r="G22" s="9">
@@ -2223,11 +2220,11 @@
       <c r="I22" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J22" s="66">
+      <c r="J22" s="64">
         <f t="shared" si="2"/>
         <v>0.24622971999999999</v>
       </c>
-      <c r="K22" s="58">
+      <c r="K22" s="56">
         <v>0.27</v>
       </c>
     </row>
@@ -2247,7 +2244,7 @@
       <c r="E23" s="9">
         <v>0.66</v>
       </c>
-      <c r="F23" s="62">
+      <c r="F23" s="60">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G23" s="9">
@@ -2259,11 +2256,11 @@
       <c r="I23" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J23" s="66">
+      <c r="J23" s="64">
         <f t="shared" si="2"/>
         <v>0.21226700000000001</v>
       </c>
-      <c r="K23" s="58">
+      <c r="K23" s="56">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
@@ -2283,7 +2280,7 @@
       <c r="E24" s="9">
         <v>0.18</v>
       </c>
-      <c r="F24" s="62">
+      <c r="F24" s="60">
         <v>99</v>
       </c>
       <c r="G24" s="9">
@@ -2295,17 +2292,17 @@
       <c r="I24" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J24" s="66">
+      <c r="J24" s="64">
         <f t="shared" si="2"/>
         <v>0.18042695</v>
       </c>
-      <c r="K24" s="58">
+      <c r="K24" s="56">
         <v>101.16</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>14</v>
@@ -2319,18 +2316,18 @@
       <c r="E25" s="9">
         <v>0.16</v>
       </c>
-      <c r="F25" s="62">
+      <c r="F25" s="60">
         <v>31.86</v>
       </c>
-      <c r="G25" s="59"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="61"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="59"/>
     </row>
     <row r="26" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>14</v>
@@ -2344,14 +2341,14 @@
       <c r="E26" s="9">
         <v>0.16</v>
       </c>
-      <c r="F26" s="63">
+      <c r="F26" s="61">
         <v>20.79</v>
       </c>
-      <c r="G26" s="59"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="61"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="58"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
     </row>
     <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
@@ -2369,7 +2366,7 @@
       <c r="E27" s="9">
         <v>2.77</v>
       </c>
-      <c r="F27" s="62">
+      <c r="F27" s="60">
         <v>0.5</v>
       </c>
       <c r="G27" s="9">
@@ -2381,11 +2378,11 @@
       <c r="I27" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J27" s="66">
+      <c r="J27" s="64">
         <f t="shared" ref="J27:J32" si="3">G27*H27</f>
         <v>0.18467229000000002</v>
       </c>
-      <c r="K27" s="58">
+      <c r="K27" s="56">
         <v>0.51</v>
       </c>
     </row>
@@ -2405,7 +2402,7 @@
       <c r="E28" s="9">
         <v>1.18</v>
       </c>
-      <c r="F28" s="62">
+      <c r="F28" s="60">
         <v>3.09</v>
       </c>
       <c r="G28" s="9">
@@ -2417,11 +2414,11 @@
       <c r="I28" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J28" s="66">
+      <c r="J28" s="64">
         <f t="shared" si="3"/>
         <v>0.12736020000000001</v>
       </c>
-      <c r="K28" s="58">
+      <c r="K28" s="56">
         <v>3.11</v>
       </c>
     </row>
@@ -2441,7 +2438,7 @@
       <c r="E29" s="9">
         <v>9.92</v>
       </c>
-      <c r="F29" s="62">
+      <c r="F29" s="60">
         <v>0.18</v>
       </c>
       <c r="G29" s="9">
@@ -2453,11 +2450,11 @@
       <c r="I29" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J29" s="66">
+      <c r="J29" s="64">
         <f t="shared" si="3"/>
         <v>4.6698740000000002E-2</v>
       </c>
-      <c r="K29" s="58">
+      <c r="K29" s="56">
         <v>0.06</v>
       </c>
     </row>
@@ -2477,7 +2474,7 @@
       <c r="E30" s="9">
         <v>10.119999999999999</v>
       </c>
-      <c r="F30" s="62">
+      <c r="F30" s="60">
         <v>0.25</v>
       </c>
       <c r="G30" s="9">
@@ -2489,11 +2486,11 @@
       <c r="I30" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J30" s="66">
+      <c r="J30" s="64">
         <f t="shared" si="3"/>
         <v>5.943476000000001E-2</v>
       </c>
-      <c r="K30" s="58">
+      <c r="K30" s="56">
         <v>0.08</v>
       </c>
     </row>
@@ -2513,7 +2510,7 @@
       <c r="E31" s="9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F31" s="62">
+      <c r="F31" s="60">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G31" s="9">
@@ -2525,11 +2522,11 @@
       <c r="I31" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J31" s="66">
+      <c r="J31" s="64">
         <f t="shared" si="3"/>
         <v>6.7925440000000004E-2</v>
       </c>
-      <c r="K31" s="58">
+      <c r="K31" s="56">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
@@ -2549,7 +2546,7 @@
       <c r="E32" s="9">
         <v>0.18</v>
       </c>
-      <c r="F32" s="62">
+      <c r="F32" s="60">
         <v>99</v>
       </c>
       <c r="G32" s="9">
@@ -2561,17 +2558,17 @@
       <c r="I32" s="4">
         <v>10.244854</v>
       </c>
-      <c r="J32" s="66">
+      <c r="J32" s="64">
         <f t="shared" si="3"/>
         <v>0.18042695</v>
       </c>
-      <c r="K32" s="58">
+      <c r="K32" s="56">
         <v>101.29</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>14</v>
@@ -2585,18 +2582,18 @@
       <c r="E33" s="9">
         <v>0.19</v>
       </c>
-      <c r="F33" s="62">
+      <c r="F33" s="60">
         <v>93.8</v>
       </c>
-      <c r="G33" s="59"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="61"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="59"/>
     </row>
     <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>14</v>
@@ -2610,14 +2607,14 @@
       <c r="E34" s="9">
         <v>0.19</v>
       </c>
-      <c r="F34" s="63">
+      <c r="F34" s="61">
         <v>60.9</v>
       </c>
-      <c r="G34" s="59"/>
-      <c r="H34" s="60"/>
-      <c r="I34" s="60"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="61"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="59"/>
     </row>
     <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
@@ -2635,7 +2632,7 @@
       <c r="E35" s="9">
         <v>37.86</v>
       </c>
-      <c r="F35" s="62">
+      <c r="F35" s="60">
         <v>0.56000000000000005</v>
       </c>
       <c r="G35" s="9">
@@ -2647,11 +2644,11 @@
       <c r="I35" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J35" s="66">
+      <c r="J35" s="64">
         <f t="shared" ref="J35:J40" si="4">G35*H35</f>
         <v>13.700800800000001</v>
       </c>
-      <c r="K35" s="58">
+      <c r="K35" s="56">
         <v>0.48</v>
       </c>
     </row>
@@ -2671,7 +2668,7 @@
       <c r="E36" s="9">
         <v>2.78</v>
       </c>
-      <c r="F36" s="62">
+      <c r="F36" s="60">
         <v>1.17</v>
       </c>
       <c r="G36" s="9">
@@ -2683,11 +2680,11 @@
       <c r="I36" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J36" s="66">
+      <c r="J36" s="64">
         <f t="shared" si="4"/>
         <v>4.4527602599999998</v>
       </c>
-      <c r="K36" s="58">
+      <c r="K36" s="56">
         <v>1.17</v>
       </c>
     </row>
@@ -2707,7 +2704,7 @@
       <c r="E37" s="9">
         <v>10.82</v>
       </c>
-      <c r="F37" s="62">
+      <c r="F37" s="60">
         <v>0.21</v>
       </c>
       <c r="G37" s="9">
@@ -2719,11 +2716,11 @@
       <c r="I37" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J37" s="66">
+      <c r="J37" s="64">
         <f t="shared" si="4"/>
         <v>6.8884581800000007</v>
       </c>
-      <c r="K37" s="58">
+      <c r="K37" s="56">
         <v>0.05</v>
       </c>
     </row>
@@ -2743,7 +2740,7 @@
       <c r="E38" s="9">
         <v>11.18</v>
       </c>
-      <c r="F38" s="62">
+      <c r="F38" s="60">
         <v>0.3</v>
       </c>
       <c r="G38" s="9">
@@ -2755,11 +2752,11 @@
       <c r="I38" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J38" s="66">
+      <c r="J38" s="64">
         <f t="shared" si="4"/>
         <v>7.3451515399999998</v>
       </c>
-      <c r="K38" s="58">
+      <c r="K38" s="56">
         <v>0.08</v>
       </c>
     </row>
@@ -2779,7 +2776,7 @@
       <c r="E39" s="9">
         <v>11.29</v>
       </c>
-      <c r="F39" s="62">
+      <c r="F39" s="60">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G39" s="9">
@@ -2791,11 +2788,11 @@
       <c r="I39" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J39" s="66">
+      <c r="J39" s="64">
         <f t="shared" si="4"/>
         <v>4.7191647200000002</v>
       </c>
-      <c r="K39" s="58">
+      <c r="K39" s="56">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
@@ -2815,7 +2812,7 @@
       <c r="E40" s="9">
         <v>2.75</v>
       </c>
-      <c r="F40" s="62">
+      <c r="F40" s="60">
         <v>101.08</v>
       </c>
       <c r="G40" s="9">
@@ -2827,17 +2824,17 @@
       <c r="I40" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J40" s="66">
+      <c r="J40" s="64">
         <f t="shared" si="4"/>
         <v>2.7782179400000002</v>
       </c>
-      <c r="K40" s="58">
+      <c r="K40" s="56">
         <v>95.82</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>15</v>
@@ -2851,18 +2848,18 @@
       <c r="E41" s="9">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F41" s="62">
+      <c r="F41" s="60">
         <v>33.159999999999997</v>
       </c>
-      <c r="G41" s="59"/>
-      <c r="H41" s="60"/>
-      <c r="I41" s="60"/>
-      <c r="J41" s="60"/>
-      <c r="K41" s="61"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="58"/>
+      <c r="J41" s="58"/>
+      <c r="K41" s="59"/>
     </row>
     <row r="42" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>15</v>
@@ -2876,14 +2873,14 @@
       <c r="E42" s="9">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F42" s="63">
+      <c r="F42" s="61">
         <v>22.18</v>
       </c>
-      <c r="G42" s="59"/>
-      <c r="H42" s="60"/>
-      <c r="I42" s="60"/>
-      <c r="J42" s="60"/>
-      <c r="K42" s="61"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="59"/>
     </row>
     <row r="43" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
@@ -2901,7 +2898,7 @@
       <c r="E43" s="9">
         <v>81.290000000000006</v>
       </c>
-      <c r="F43" s="62">
+      <c r="F43" s="60">
         <v>0.48</v>
       </c>
       <c r="G43" s="9">
@@ -2913,11 +2910,11 @@
       <c r="I43" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J43" s="66">
+      <c r="J43" s="64">
         <f t="shared" ref="J43:J48" si="5">G43*H43</f>
         <v>4.5288758199999997</v>
       </c>
-      <c r="K43" s="58">
+      <c r="K43" s="56">
         <v>0.49</v>
       </c>
     </row>
@@ -2937,7 +2934,7 @@
       <c r="E44" s="9">
         <v>2.78</v>
       </c>
-      <c r="F44" s="62">
+      <c r="F44" s="60">
         <v>2.95</v>
       </c>
       <c r="G44" s="9">
@@ -2949,11 +2946,11 @@
       <c r="I44" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J44" s="66">
+      <c r="J44" s="64">
         <f t="shared" si="5"/>
         <v>4.4527602599999998</v>
       </c>
-      <c r="K44" s="58">
+      <c r="K44" s="56">
         <v>2.96</v>
       </c>
     </row>
@@ -2973,7 +2970,7 @@
       <c r="E45" s="9">
         <v>6.05</v>
       </c>
-      <c r="F45" s="62">
+      <c r="F45" s="60">
         <v>0.02</v>
       </c>
       <c r="G45" s="9">
@@ -2985,11 +2982,11 @@
       <c r="I45" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J45" s="66">
+      <c r="J45" s="64">
         <f t="shared" si="5"/>
         <v>5.1758580800000002</v>
       </c>
-      <c r="K45" s="58">
+      <c r="K45" s="56">
         <v>0.1</v>
       </c>
     </row>
@@ -3009,7 +3006,7 @@
       <c r="E46" s="9">
         <v>4.6900000000000004</v>
       </c>
-      <c r="F46" s="62">
+      <c r="F46" s="60">
         <v>0.02</v>
       </c>
       <c r="G46" s="9">
@@ -3021,11 +3018,11 @@
       <c r="I46" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J46" s="66">
+      <c r="J46" s="64">
         <f t="shared" si="5"/>
         <v>6.2414759200000001</v>
       </c>
-      <c r="K46" s="58">
+      <c r="K46" s="56">
         <v>0.19</v>
       </c>
     </row>
@@ -3045,7 +3042,7 @@
       <c r="E47" s="9">
         <v>4.63</v>
       </c>
-      <c r="F47" s="62">
+      <c r="F47" s="60">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="G47" s="9">
@@ -3057,11 +3054,11 @@
       <c r="I47" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J47" s="66">
+      <c r="J47" s="64">
         <f t="shared" si="5"/>
         <v>4.1863558000000003</v>
       </c>
-      <c r="K47" s="58">
+      <c r="K47" s="56">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -3081,7 +3078,7 @@
       <c r="E48" s="9">
         <v>2.75</v>
       </c>
-      <c r="F48" s="62">
+      <c r="F48" s="60">
         <v>95.9</v>
       </c>
       <c r="G48" s="9">
@@ -3093,17 +3090,17 @@
       <c r="I48" s="4">
         <v>14.050458000000001</v>
       </c>
-      <c r="J48" s="66">
+      <c r="J48" s="64">
         <f t="shared" si="5"/>
         <v>2.7782179400000002</v>
       </c>
-      <c r="K48" s="58">
+      <c r="K48" s="56">
         <v>95.8</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>15</v>
@@ -3117,18 +3114,18 @@
       <c r="E49" s="9">
         <v>4.71</v>
       </c>
-      <c r="F49" s="62">
+      <c r="F49" s="60">
         <v>92.8</v>
       </c>
-      <c r="G49" s="59"/>
-      <c r="H49" s="60"/>
-      <c r="I49" s="60"/>
-      <c r="J49" s="60"/>
-      <c r="K49" s="61"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="58"/>
+      <c r="I49" s="58"/>
+      <c r="J49" s="58"/>
+      <c r="K49" s="59"/>
     </row>
     <row r="50" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>15</v>
@@ -3142,14 +3139,14 @@
       <c r="E50" s="9">
         <v>4.71</v>
       </c>
-      <c r="F50" s="63">
+      <c r="F50" s="61">
         <v>57.93</v>
       </c>
-      <c r="G50" s="59"/>
-      <c r="H50" s="60"/>
-      <c r="I50" s="60"/>
-      <c r="J50" s="60"/>
-      <c r="K50" s="61"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="58"/>
+      <c r="J50" s="58"/>
+      <c r="K50" s="59"/>
     </row>
     <row r="51" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
@@ -3167,7 +3164,7 @@
       <c r="E51" s="9">
         <v>903.48</v>
       </c>
-      <c r="F51" s="62">
+      <c r="F51" s="60">
         <v>0.28999999999999998</v>
       </c>
       <c r="G51" s="9">
@@ -3179,11 +3176,11 @@
       <c r="I51" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J51" s="66">
+      <c r="J51" s="64">
         <f t="shared" ref="J51:J56" si="6">G51*H51</f>
         <v>952.69226313000013</v>
       </c>
-      <c r="K51" s="58">
+      <c r="K51" s="56">
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -3203,7 +3200,7 @@
       <c r="E52" s="10">
         <v>1090000000000</v>
       </c>
-      <c r="F52" s="62">
+      <c r="F52" s="60">
         <v>0.71</v>
       </c>
       <c r="G52" s="9">
@@ -3215,11 +3212,11 @@
       <c r="I52" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J52" s="66">
+      <c r="J52" s="64">
         <f t="shared" si="6"/>
         <v>383.44875321000001</v>
       </c>
-      <c r="K52" s="58">
+      <c r="K52" s="56">
         <v>0.69</v>
       </c>
     </row>
@@ -3239,7 +3236,7 @@
       <c r="E53" s="9">
         <v>396.4</v>
       </c>
-      <c r="F53" s="62">
+      <c r="F53" s="60">
         <v>0.1</v>
       </c>
       <c r="G53" s="9">
@@ -3251,11 +3248,11 @@
       <c r="I53" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J53" s="66">
+      <c r="J53" s="64">
         <f t="shared" si="6"/>
         <v>419.02647258000002</v>
       </c>
-      <c r="K53" s="58">
+      <c r="K53" s="56">
         <v>0.11</v>
       </c>
     </row>
@@ -3275,7 +3272,7 @@
       <c r="E54" s="9">
         <v>845.52</v>
       </c>
-      <c r="F54" s="62">
+      <c r="F54" s="60">
         <v>0.18</v>
       </c>
       <c r="G54" s="9">
@@ -3287,11 +3284,11 @@
       <c r="I54" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J54" s="66">
+      <c r="J54" s="64">
         <f t="shared" si="6"/>
         <v>422.97955251000002</v>
       </c>
-      <c r="K54" s="58">
+      <c r="K54" s="56">
         <v>0.26</v>
       </c>
     </row>
@@ -3311,7 +3308,7 @@
       <c r="E55" s="9">
         <v>1090.3499999999999</v>
       </c>
-      <c r="F55" s="62">
+      <c r="F55" s="60">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G55" s="9">
@@ -3323,11 +3320,11 @@
       <c r="I55" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J55" s="66">
+      <c r="J55" s="64">
         <f t="shared" si="6"/>
         <v>347.87103384</v>
       </c>
-      <c r="K55" s="58">
+      <c r="K55" s="56">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -3347,7 +3344,7 @@
       <c r="E56" s="9">
         <v>536.14</v>
       </c>
-      <c r="F56" s="62">
+      <c r="F56" s="60">
         <v>47.79</v>
       </c>
       <c r="G56" s="9">
@@ -3359,17 +3356,17 @@
       <c r="I56" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J56" s="66">
+      <c r="J56" s="64">
         <f t="shared" si="6"/>
         <v>537.61887048000006</v>
       </c>
-      <c r="K56" s="58">
+      <c r="K56" s="56">
         <v>48.41</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>16</v>
@@ -3383,18 +3380,18 @@
       <c r="E57" s="9">
         <v>212.97</v>
       </c>
-      <c r="F57" s="62">
+      <c r="F57" s="60">
         <v>14.67</v>
       </c>
-      <c r="G57" s="59"/>
-      <c r="H57" s="60"/>
-      <c r="I57" s="60"/>
-      <c r="J57" s="60"/>
-      <c r="K57" s="61"/>
+      <c r="G57" s="57"/>
+      <c r="H57" s="58"/>
+      <c r="I57" s="58"/>
+      <c r="J57" s="58"/>
+      <c r="K57" s="59"/>
     </row>
     <row r="58" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>16</v>
@@ -3408,14 +3405,14 @@
       <c r="E58" s="9">
         <v>212.97</v>
       </c>
-      <c r="F58" s="63">
+      <c r="F58" s="61">
         <v>10.52</v>
       </c>
-      <c r="G58" s="59"/>
-      <c r="H58" s="60"/>
-      <c r="I58" s="60"/>
-      <c r="J58" s="60"/>
-      <c r="K58" s="61"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="58"/>
+      <c r="I58" s="58"/>
+      <c r="J58" s="58"/>
+      <c r="K58" s="59"/>
     </row>
     <row r="59" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
@@ -3433,7 +3430,7 @@
       <c r="E59" s="9">
         <v>739.84</v>
       </c>
-      <c r="F59" s="62">
+      <c r="F59" s="60">
         <v>0.32</v>
       </c>
       <c r="G59" s="9">
@@ -3445,11 +3442,11 @@
       <c r="I59" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J59" s="66">
+      <c r="J59" s="64">
         <f t="shared" ref="J59:J64" si="7">G59*H59</f>
         <v>747.13210676999995</v>
       </c>
-      <c r="K59" s="58">
+      <c r="K59" s="56">
         <v>0.3</v>
       </c>
     </row>
@@ -3469,7 +3466,7 @@
       <c r="E60" s="10">
         <v>1090000000000</v>
       </c>
-      <c r="F60" s="62">
+      <c r="F60" s="60">
         <v>1.79</v>
       </c>
       <c r="G60" s="9">
@@ -3481,11 +3478,11 @@
       <c r="I60" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J60" s="66">
+      <c r="J60" s="64">
         <f t="shared" si="7"/>
         <v>383.44875321000001</v>
       </c>
-      <c r="K60" s="58">
+      <c r="K60" s="56">
         <v>1.78</v>
       </c>
     </row>
@@ -3505,7 +3502,7 @@
       <c r="E61" s="9">
         <v>249.74</v>
       </c>
-      <c r="F61" s="62">
+      <c r="F61" s="60">
         <v>0.05</v>
       </c>
       <c r="G61" s="9">
@@ -3517,11 +3514,11 @@
       <c r="I61" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J61" s="66">
+      <c r="J61" s="64">
         <f t="shared" si="7"/>
         <v>252.99711552000002</v>
       </c>
-      <c r="K61" s="58">
+      <c r="K61" s="56">
         <v>0.03</v>
       </c>
     </row>
@@ -3541,7 +3538,7 @@
       <c r="E62" s="9">
         <v>645.32000000000005</v>
       </c>
-      <c r="F62" s="62">
+      <c r="F62" s="60">
         <v>0.32</v>
       </c>
       <c r="G62" s="9">
@@ -3553,11 +3550,11 @@
       <c r="I62" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J62" s="66">
+      <c r="J62" s="64">
         <f t="shared" si="7"/>
         <v>383.44875321000001</v>
       </c>
-      <c r="K62" s="58">
+      <c r="K62" s="56">
         <v>0.24</v>
       </c>
     </row>
@@ -3577,7 +3574,7 @@
       <c r="E63" s="9">
         <v>381.2</v>
       </c>
-      <c r="F63" s="62">
+      <c r="F63" s="60">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="G63" s="9">
@@ -3589,11 +3586,11 @@
       <c r="I63" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J63" s="66">
+      <c r="J63" s="64">
         <f t="shared" si="7"/>
         <v>272.76251516999997</v>
       </c>
-      <c r="K63" s="58">
+      <c r="K63" s="56">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -3613,7 +3610,7 @@
       <c r="E64" s="9">
         <v>536.14</v>
       </c>
-      <c r="F64" s="62">
+      <c r="F64" s="60">
         <v>48.09</v>
       </c>
       <c r="G64" s="9">
@@ -3625,17 +3622,17 @@
       <c r="I64" s="4">
         <v>646.36959999999999</v>
       </c>
-      <c r="J64" s="66">
+      <c r="J64" s="64">
         <f t="shared" si="7"/>
         <v>537.61887048000006</v>
       </c>
-      <c r="K64" s="58">
+      <c r="K64" s="56">
         <v>47.92</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>16</v>
@@ -3649,18 +3646,18 @@
       <c r="E65" s="9">
         <v>202.42</v>
       </c>
-      <c r="F65" s="62">
+      <c r="F65" s="60">
         <v>42.22</v>
       </c>
-      <c r="G65" s="59"/>
-      <c r="H65" s="60"/>
-      <c r="I65" s="60"/>
-      <c r="J65" s="60"/>
-      <c r="K65" s="61"/>
+      <c r="G65" s="57"/>
+      <c r="H65" s="58"/>
+      <c r="I65" s="58"/>
+      <c r="J65" s="58"/>
+      <c r="K65" s="59"/>
     </row>
     <row r="66" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>16</v>
@@ -3674,14 +3671,14 @@
       <c r="E66" s="9">
         <v>202.42</v>
       </c>
-      <c r="F66" s="63">
+      <c r="F66" s="61">
         <v>28.41</v>
       </c>
-      <c r="G66" s="59"/>
-      <c r="H66" s="60"/>
-      <c r="I66" s="60"/>
-      <c r="J66" s="60"/>
-      <c r="K66" s="61"/>
+      <c r="G66" s="57"/>
+      <c r="H66" s="58"/>
+      <c r="I66" s="58"/>
+      <c r="J66" s="58"/>
+      <c r="K66" s="59"/>
     </row>
     <row r="67" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
@@ -3699,7 +3696,7 @@
       <c r="E67" s="9">
         <v>3888.78</v>
       </c>
-      <c r="F67" s="62">
+      <c r="F67" s="60">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G67" s="9">
@@ -3711,11 +3708,11 @@
       <c r="I67" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J67" s="66">
+      <c r="J67" s="64">
         <f t="shared" ref="J67:J72" si="8">G67*H67</f>
         <v>25.730280160000003</v>
       </c>
-      <c r="K67" s="58">
+      <c r="K67" s="56">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -3735,7 +3732,7 @@
       <c r="E68" s="9">
         <v>33.29</v>
       </c>
-      <c r="F68" s="62">
+      <c r="F68" s="60">
         <v>0.28000000000000003</v>
       </c>
       <c r="G68" s="9">
@@ -3747,11 +3744,11 @@
       <c r="I68" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J68" s="66">
+      <c r="J68" s="64">
         <f t="shared" si="8"/>
         <v>7.1662584000000011</v>
       </c>
-      <c r="K68" s="58">
+      <c r="K68" s="56">
         <v>0.28000000000000003</v>
       </c>
     </row>
@@ -3771,7 +3768,7 @@
       <c r="E69" s="9">
         <v>366.78</v>
       </c>
-      <c r="F69" s="62">
+      <c r="F69" s="60">
         <v>0.09</v>
       </c>
       <c r="G69" s="9">
@@ -3783,11 +3780,11 @@
       <c r="I69" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J69" s="66">
+      <c r="J69" s="64">
         <f t="shared" si="8"/>
         <v>5.5282564800000005</v>
       </c>
-      <c r="K69" s="58">
+      <c r="K69" s="56">
         <v>0.02</v>
       </c>
     </row>
@@ -3807,7 +3804,7 @@
       <c r="E70" s="9">
         <v>366.74</v>
       </c>
-      <c r="F70" s="62">
+      <c r="F70" s="60">
         <v>0.13</v>
       </c>
       <c r="G70" s="9">
@@ -3819,11 +3816,11 @@
       <c r="I70" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J70" s="66">
+      <c r="J70" s="64">
         <f t="shared" si="8"/>
         <v>5.3235062400000004</v>
       </c>
-      <c r="K70" s="58">
+      <c r="K70" s="56">
         <v>0.05</v>
       </c>
     </row>
@@ -3843,7 +3840,7 @@
       <c r="E71" s="9">
         <v>4.32</v>
       </c>
-      <c r="F71" s="62">
+      <c r="F71" s="60">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="G71" s="9">
@@ -3855,11 +3852,11 @@
       <c r="I71" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J71" s="66">
+      <c r="J71" s="64">
         <f t="shared" si="8"/>
         <v>4.5727553600000004</v>
       </c>
-      <c r="K71" s="58">
+      <c r="K71" s="56">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -3879,7 +3876,7 @@
       <c r="E72" s="9">
         <v>10.19</v>
       </c>
-      <c r="F72" s="62">
+      <c r="F72" s="60">
         <v>9.94</v>
       </c>
       <c r="G72" s="9">
@@ -3891,17 +3888,17 @@
       <c r="I72" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J72" s="66">
+      <c r="J72" s="64">
         <f t="shared" si="8"/>
         <v>10.16926192</v>
       </c>
-      <c r="K72" s="58">
+      <c r="K72" s="56">
         <v>9.85</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>17</v>
@@ -3915,18 +3912,18 @@
       <c r="E73" s="9">
         <v>1.17</v>
       </c>
-      <c r="F73" s="62">
+      <c r="F73" s="60">
         <v>3.02</v>
       </c>
-      <c r="G73" s="59"/>
-      <c r="H73" s="60"/>
-      <c r="I73" s="60"/>
-      <c r="J73" s="60"/>
-      <c r="K73" s="61"/>
+      <c r="G73" s="57"/>
+      <c r="H73" s="58"/>
+      <c r="I73" s="58"/>
+      <c r="J73" s="58"/>
+      <c r="K73" s="59"/>
     </row>
     <row r="74" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>17</v>
@@ -3940,14 +3937,14 @@
       <c r="E74" s="9">
         <v>1.17</v>
       </c>
-      <c r="F74" s="63">
+      <c r="F74" s="61">
         <v>4.7699999999999996</v>
       </c>
-      <c r="G74" s="59"/>
-      <c r="H74" s="60"/>
-      <c r="I74" s="60"/>
-      <c r="J74" s="60"/>
-      <c r="K74" s="61"/>
+      <c r="G74" s="57"/>
+      <c r="H74" s="58"/>
+      <c r="I74" s="58"/>
+      <c r="J74" s="58"/>
+      <c r="K74" s="59"/>
     </row>
     <row r="75" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
@@ -3965,7 +3962,7 @@
       <c r="E75" s="9">
         <v>1587.31</v>
       </c>
-      <c r="F75" s="62">
+      <c r="F75" s="60">
         <v>0.08</v>
       </c>
       <c r="G75" s="9">
@@ -3977,11 +3974,11 @@
       <c r="I75" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J75" s="66">
+      <c r="J75" s="64">
         <f t="shared" ref="J75:J80" si="9">G75*H75</f>
         <v>9.7597614400000001</v>
       </c>
-      <c r="K75" s="58">
+      <c r="K75" s="56">
         <v>0.08</v>
       </c>
     </row>
@@ -4001,7 +3998,7 @@
       <c r="E76" s="9">
         <v>33.29</v>
       </c>
-      <c r="F76" s="62">
+      <c r="F76" s="60">
         <v>0.71</v>
       </c>
       <c r="G76" s="9">
@@ -4013,11 +4010,11 @@
       <c r="I76" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J76" s="66">
+      <c r="J76" s="64">
         <f t="shared" si="9"/>
         <v>7.1662584000000011</v>
       </c>
-      <c r="K76" s="58">
+      <c r="K76" s="56">
         <v>0.7</v>
       </c>
     </row>
@@ -4037,7 +4034,7 @@
       <c r="E77" s="9">
         <v>28.62</v>
       </c>
-      <c r="F77" s="62">
+      <c r="F77" s="60">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G77" s="9">
@@ -4049,11 +4046,11 @@
       <c r="I77" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J77" s="66">
+      <c r="J77" s="64">
         <f t="shared" si="9"/>
         <v>6.1425072000000007</v>
       </c>
-      <c r="K77" s="58">
+      <c r="K77" s="56">
         <v>0.02</v>
       </c>
     </row>
@@ -4073,7 +4070,7 @@
       <c r="E78" s="9">
         <v>6.49</v>
       </c>
-      <c r="F78" s="62">
+      <c r="F78" s="60">
         <v>0.04</v>
       </c>
       <c r="G78" s="9">
@@ -4085,11 +4082,11 @@
       <c r="I78" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J78" s="66">
+      <c r="J78" s="64">
         <f t="shared" si="9"/>
         <v>6.0060070400000001</v>
       </c>
-      <c r="K78" s="58">
+      <c r="K78" s="56">
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -4109,7 +4106,7 @@
       <c r="E79" s="9">
         <v>6.13</v>
       </c>
-      <c r="F79" s="62">
+      <c r="F79" s="60">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="G79" s="9">
@@ -4121,11 +4118,11 @@
       <c r="I79" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J79" s="66">
+      <c r="J79" s="64">
         <f t="shared" si="9"/>
         <v>5.3235062400000004</v>
       </c>
-      <c r="K79" s="58">
+      <c r="K79" s="56">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -4145,7 +4142,7 @@
       <c r="E80" s="9">
         <v>10.19</v>
       </c>
-      <c r="F80" s="62">
+      <c r="F80" s="60">
         <v>9.9700000000000006</v>
       </c>
       <c r="G80" s="9">
@@ -4157,17 +4154,17 @@
       <c r="I80" s="4">
         <v>363.74403000000001</v>
       </c>
-      <c r="J80" s="66">
+      <c r="J80" s="64">
         <f t="shared" si="9"/>
         <v>10.16926192</v>
       </c>
-      <c r="K80" s="58">
+      <c r="K80" s="56">
         <v>9.92</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>17</v>
@@ -4181,18 +4178,18 @@
       <c r="E81" s="9">
         <v>1.51</v>
       </c>
-      <c r="F81" s="62">
+      <c r="F81" s="60">
         <v>13.7</v>
       </c>
-      <c r="G81" s="59"/>
-      <c r="H81" s="60"/>
-      <c r="I81" s="60"/>
-      <c r="J81" s="60"/>
-      <c r="K81" s="61"/>
+      <c r="G81" s="57"/>
+      <c r="H81" s="58"/>
+      <c r="I81" s="58"/>
+      <c r="J81" s="58"/>
+      <c r="K81" s="59"/>
     </row>
     <row r="82" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>17</v>
@@ -4206,14 +4203,14 @@
       <c r="E82" s="9">
         <v>1.51</v>
       </c>
-      <c r="F82" s="63">
+      <c r="F82" s="61">
         <v>12.4</v>
       </c>
-      <c r="G82" s="59"/>
-      <c r="H82" s="60"/>
-      <c r="I82" s="60"/>
-      <c r="J82" s="60"/>
-      <c r="K82" s="61"/>
+      <c r="G82" s="57"/>
+      <c r="H82" s="58"/>
+      <c r="I82" s="58"/>
+      <c r="J82" s="58"/>
+      <c r="K82" s="59"/>
     </row>
     <row r="83" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="18" t="s">
@@ -4225,16 +4222,16 @@
       <c r="C83" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D83" s="62">
+      <c r="D83" s="60">
         <v>3</v>
       </c>
       <c r="E83" s="9">
         <v>274.10000000000002</v>
       </c>
-      <c r="F83" s="62">
+      <c r="F83" s="60">
         <v>2.12</v>
       </c>
-      <c r="G83" s="65">
+      <c r="G83" s="63">
         <v>1.68</v>
       </c>
       <c r="H83" s="4">
@@ -4243,11 +4240,11 @@
       <c r="I83" s="4">
         <v>0.119245</v>
       </c>
-      <c r="J83" s="66">
+      <c r="J83" s="64">
         <f t="shared" ref="J83:J87" si="10">G83*H83</f>
         <v>8.7583221600000005</v>
       </c>
-      <c r="K83" s="58">
+      <c r="K83" s="56">
         <v>2.0699999999999998</v>
       </c>
     </row>
@@ -4261,13 +4258,13 @@
       <c r="C84" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D84" s="62">
+      <c r="D84" s="60">
         <v>3</v>
       </c>
       <c r="E84" s="9">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F84" s="62">
+      <c r="F84" s="60">
         <v>4.37</v>
       </c>
       <c r="G84" s="9">
@@ -4279,11 +4276,11 @@
       <c r="I84" s="4">
         <v>0.119245</v>
       </c>
-      <c r="J84" s="66">
+      <c r="J84" s="64">
         <f t="shared" si="10"/>
         <v>4.0663638600000001</v>
       </c>
-      <c r="K84" s="58">
+      <c r="K84" s="56">
         <v>4.37</v>
       </c>
     </row>
@@ -4297,13 +4294,13 @@
       <c r="C85" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D85" s="62">
+      <c r="D85" s="60">
         <v>3</v>
       </c>
       <c r="E85" s="9">
         <v>4.0199999999999996</v>
       </c>
-      <c r="F85" s="62">
+      <c r="F85" s="60">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="G85" s="9">
@@ -4315,11 +4312,11 @@
       <c r="I85" s="4">
         <v>0.119245</v>
       </c>
-      <c r="J85" s="66">
+      <c r="J85" s="64">
         <f t="shared" si="10"/>
         <v>3.70143377</v>
       </c>
-      <c r="K85" s="58">
+      <c r="K85" s="56">
         <v>2.4E-2</v>
       </c>
     </row>
@@ -4333,7 +4330,7 @@
       <c r="C86" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D86" s="62">
+      <c r="D86" s="60">
         <v>3</v>
       </c>
       <c r="E86" s="9">
@@ -4351,11 +4348,11 @@
       <c r="I86" s="4">
         <v>0.119245</v>
       </c>
-      <c r="J86" s="66">
+      <c r="J86" s="64">
         <f t="shared" si="10"/>
         <v>4.0663638600000001</v>
       </c>
-      <c r="K86" s="58">
+      <c r="K86" s="56">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
@@ -4369,7 +4366,7 @@
       <c r="C87" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D87" s="62">
+      <c r="D87" s="60">
         <v>3</v>
       </c>
       <c r="E87" s="9">
@@ -4387,11 +4384,11 @@
       <c r="I87" s="4">
         <v>0.119245</v>
       </c>
-      <c r="J87" s="66">
+      <c r="J87" s="64">
         <f t="shared" si="10"/>
         <v>4.1184967300000004</v>
       </c>
-      <c r="K87" s="58">
+      <c r="K87" s="56">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
@@ -4405,20 +4402,20 @@
       <c r="C88" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D88" s="62">
-        <v>3</v>
-      </c>
-      <c r="E88" s="133"/>
-      <c r="F88" s="134"/>
-      <c r="G88" s="133"/>
-      <c r="H88" s="135"/>
-      <c r="I88" s="135"/>
-      <c r="J88" s="135"/>
-      <c r="K88" s="136"/>
+      <c r="D88" s="60">
+        <v>3</v>
+      </c>
+      <c r="E88" s="118"/>
+      <c r="F88" s="119"/>
+      <c r="G88" s="118"/>
+      <c r="H88" s="120"/>
+      <c r="I88" s="120"/>
+      <c r="J88" s="120"/>
+      <c r="K88" s="121"/>
     </row>
     <row r="89" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B89" s="19" t="s">
         <v>19</v>
@@ -4426,24 +4423,24 @@
       <c r="C89" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D89" s="62">
-        <v>3</v>
-      </c>
-      <c r="E89" s="67">
+      <c r="D89" s="60">
+        <v>3</v>
+      </c>
+      <c r="E89" s="65">
         <v>4.37</v>
       </c>
-      <c r="F89" s="62">
+      <c r="F89" s="60">
         <v>84.58</v>
       </c>
-      <c r="G89" s="59"/>
-      <c r="H89" s="60"/>
-      <c r="I89" s="60"/>
-      <c r="J89" s="60"/>
-      <c r="K89" s="61"/>
+      <c r="G89" s="57"/>
+      <c r="H89" s="58"/>
+      <c r="I89" s="58"/>
+      <c r="J89" s="58"/>
+      <c r="K89" s="59"/>
     </row>
     <row r="90" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B90" s="19" t="s">
         <v>19</v>
@@ -4451,20 +4448,20 @@
       <c r="C90" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D90" s="62">
-        <v>3</v>
-      </c>
-      <c r="E90" s="67">
+      <c r="D90" s="60">
+        <v>3</v>
+      </c>
+      <c r="E90" s="65">
         <v>4.37</v>
       </c>
-      <c r="F90" s="63">
+      <c r="F90" s="61">
         <v>54.07</v>
       </c>
-      <c r="G90" s="59"/>
-      <c r="H90" s="60"/>
-      <c r="I90" s="60"/>
-      <c r="J90" s="60"/>
-      <c r="K90" s="61"/>
+      <c r="G90" s="57"/>
+      <c r="H90" s="58"/>
+      <c r="I90" s="58"/>
+      <c r="J90" s="58"/>
+      <c r="K90" s="59"/>
     </row>
     <row r="91" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="18" t="s">
@@ -4476,7 +4473,7 @@
       <c r="C91" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D91" s="62">
+      <c r="D91" s="60">
         <v>9</v>
       </c>
       <c r="E91" s="9">
@@ -4494,11 +4491,11 @@
       <c r="I91" s="4">
         <v>0.119245</v>
       </c>
-      <c r="J91" s="66">
+      <c r="J91" s="64">
         <f t="shared" ref="J91:J95" si="11">G91*H91</f>
         <v>10.16590965</v>
       </c>
-      <c r="K91" s="58">
+      <c r="K91" s="56">
         <v>2.35</v>
       </c>
     </row>
@@ -4512,7 +4509,7 @@
       <c r="C92" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D92" s="62">
+      <c r="D92" s="60">
         <v>9</v>
       </c>
       <c r="E92" s="9">
@@ -4530,11 +4527,11 @@
       <c r="I92" s="4">
         <v>0.119245</v>
       </c>
-      <c r="J92" s="66">
+      <c r="J92" s="64">
         <f t="shared" si="11"/>
         <v>4.0663638600000001</v>
       </c>
-      <c r="K92" s="58">
+      <c r="K92" s="56">
         <v>11.1</v>
       </c>
     </row>
@@ -4548,7 +4545,7 @@
       <c r="C93" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D93" s="62">
+      <c r="D93" s="60">
         <v>9</v>
       </c>
       <c r="E93" s="9">
@@ -4566,11 +4563,11 @@
       <c r="I93" s="4">
         <v>0.119245</v>
       </c>
-      <c r="J93" s="66">
+      <c r="J93" s="64">
         <f t="shared" si="11"/>
         <v>3.9099652499999999</v>
       </c>
-      <c r="K93" s="58">
+      <c r="K93" s="56">
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
@@ -4584,7 +4581,7 @@
       <c r="C94" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D94" s="62">
+      <c r="D94" s="60">
         <v>9</v>
       </c>
       <c r="E94" s="9">
@@ -4602,11 +4599,11 @@
       <c r="I94" s="4">
         <v>0.119245</v>
       </c>
-      <c r="J94" s="66">
+      <c r="J94" s="64">
         <f t="shared" si="11"/>
         <v>3.8578323800000001</v>
       </c>
-      <c r="K94" s="58">
+      <c r="K94" s="56">
         <v>6.3E-2</v>
       </c>
     </row>
@@ -4620,7 +4617,7 @@
       <c r="C95" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D95" s="62">
+      <c r="D95" s="60">
         <v>9</v>
       </c>
       <c r="E95" s="9">
@@ -4638,11 +4635,11 @@
       <c r="I95" s="4">
         <v>0.119245</v>
       </c>
-      <c r="J95" s="66">
+      <c r="J95" s="64">
         <f t="shared" si="11"/>
         <v>4.3270282099999999</v>
       </c>
-      <c r="K95" s="58">
+      <c r="K95" s="56">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -4656,20 +4653,20 @@
       <c r="C96" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D96" s="62">
+      <c r="D96" s="60">
         <v>9</v>
       </c>
-      <c r="E96" s="133"/>
-      <c r="F96" s="134"/>
-      <c r="G96" s="133"/>
-      <c r="H96" s="135"/>
-      <c r="I96" s="135"/>
-      <c r="J96" s="135"/>
-      <c r="K96" s="136"/>
+      <c r="E96" s="118"/>
+      <c r="F96" s="119"/>
+      <c r="G96" s="118"/>
+      <c r="H96" s="120"/>
+      <c r="I96" s="120"/>
+      <c r="J96" s="120"/>
+      <c r="K96" s="121"/>
     </row>
     <row r="97" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B97" s="19" t="s">
         <v>19</v>
@@ -4677,24 +4674,24 @@
       <c r="C97" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D97" s="62">
+      <c r="D97" s="60">
         <v>9</v>
       </c>
-      <c r="E97" s="67">
+      <c r="E97" s="65">
         <v>3.3</v>
       </c>
-      <c r="F97" s="62">
+      <c r="F97" s="60">
         <v>265.18</v>
       </c>
-      <c r="G97" s="59"/>
-      <c r="H97" s="60"/>
-      <c r="I97" s="60"/>
-      <c r="J97" s="60"/>
-      <c r="K97" s="61"/>
+      <c r="G97" s="57"/>
+      <c r="H97" s="58"/>
+      <c r="I97" s="58"/>
+      <c r="J97" s="58"/>
+      <c r="K97" s="59"/>
     </row>
     <row r="98" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B98" s="19" t="s">
         <v>19</v>
@@ -4702,20 +4699,20 @@
       <c r="C98" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D98" s="62">
+      <c r="D98" s="60">
         <v>9</v>
       </c>
-      <c r="E98" s="67">
+      <c r="E98" s="65">
         <v>3.3</v>
       </c>
-      <c r="F98" s="78">
+      <c r="F98" s="76">
         <v>155.9</v>
       </c>
-      <c r="G98" s="59"/>
-      <c r="H98" s="60"/>
-      <c r="I98" s="60"/>
-      <c r="J98" s="60"/>
-      <c r="K98" s="61"/>
+      <c r="G98" s="57"/>
+      <c r="H98" s="58"/>
+      <c r="I98" s="58"/>
+      <c r="J98" s="58"/>
+      <c r="K98" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4748,514 +4745,514 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70"/>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="104" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="104" t="s">
+      <c r="A1" s="68"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="108"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="125" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="127"/>
     </row>
     <row r="2" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="126" t="s">
+      <c r="C2" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="127" t="s">
+      <c r="D2" s="112" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="128" t="s">
+      <c r="F2" s="113" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="128" t="s">
+      <c r="G2" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="128" t="s">
+      <c r="H2" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="129" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="130" t="s">
+      <c r="I2" s="115" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="116" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="131" t="s">
+      <c r="K2" s="116" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="131" t="s">
+      <c r="L2" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="132" t="s">
+    </row>
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="100" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="115" t="s">
+      <c r="B3" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="102">
+        <v>49</v>
+      </c>
+      <c r="D3" s="103">
+        <v>7.44</v>
+      </c>
+      <c r="E3" s="104">
+        <v>51.39</v>
+      </c>
+      <c r="F3" s="104">
+        <v>19.98</v>
+      </c>
+      <c r="G3" s="104">
+        <v>17.55</v>
+      </c>
+      <c r="H3" s="105">
+        <v>3.64</v>
+      </c>
+      <c r="I3" s="106">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="J3" s="107">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="K3" s="107">
+        <v>5.9</v>
+      </c>
+      <c r="L3" s="108">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="116" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="117">
-        <v>49</v>
-      </c>
-      <c r="D3" s="118">
-        <v>7.44</v>
-      </c>
-      <c r="E3" s="119">
-        <v>51.39</v>
-      </c>
-      <c r="F3" s="119">
-        <v>19.98</v>
-      </c>
-      <c r="G3" s="119">
-        <v>17.55</v>
-      </c>
-      <c r="H3" s="120">
-        <v>3.64</v>
-      </c>
-      <c r="I3" s="121">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="J3" s="122">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="K3" s="122">
+      <c r="B4" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="95">
+        <v>9</v>
+      </c>
+      <c r="D4" s="82">
+        <v>9.61</v>
+      </c>
+      <c r="E4" s="70">
+        <v>63.86</v>
+      </c>
+      <c r="F4" s="70">
+        <v>12.76</v>
+      </c>
+      <c r="G4" s="70">
+        <v>13.01</v>
+      </c>
+      <c r="H4" s="83">
+        <v>0.75</v>
+      </c>
+      <c r="I4" s="87">
+        <v>27</v>
+      </c>
+      <c r="J4" s="71">
+        <v>27</v>
+      </c>
+      <c r="K4" s="71">
+        <v>78</v>
+      </c>
+      <c r="L4" s="88">
+        <v>48.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="96" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="95">
+        <v>9</v>
+      </c>
+      <c r="D5" s="82">
+        <v>4.41</v>
+      </c>
+      <c r="E5" s="70">
+        <v>45.24</v>
+      </c>
+      <c r="F5" s="70">
+        <v>23.74</v>
+      </c>
+      <c r="G5" s="70">
+        <v>25.3</v>
+      </c>
+      <c r="H5" s="83">
+        <v>1.31</v>
+      </c>
+      <c r="I5" s="87">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J5" s="71">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K5" s="71">
+        <v>5.5</v>
+      </c>
+      <c r="L5" s="88">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="95">
+        <v>9</v>
+      </c>
+      <c r="D6" s="82">
+        <v>7.52</v>
+      </c>
+      <c r="E6" s="70">
+        <v>69.650000000000006</v>
+      </c>
+      <c r="F6" s="70">
+        <v>10.69</v>
+      </c>
+      <c r="G6" s="70">
+        <v>11.27</v>
+      </c>
+      <c r="H6" s="83">
+        <v>0.87</v>
+      </c>
+      <c r="I6" s="87">
+        <v>15.6</v>
+      </c>
+      <c r="J6" s="71">
+        <v>15.6</v>
+      </c>
+      <c r="K6" s="71">
+        <v>35</v>
+      </c>
+      <c r="L6" s="88">
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="94" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="95">
+        <v>9</v>
+      </c>
+      <c r="D7" s="82">
+        <v>10.84</v>
+      </c>
+      <c r="E7" s="70">
+        <v>66.67</v>
+      </c>
+      <c r="F7" s="70">
+        <v>9.57</v>
+      </c>
+      <c r="G7" s="70">
+        <v>12.12</v>
+      </c>
+      <c r="H7" s="83">
+        <v>0.8</v>
+      </c>
+      <c r="I7" s="87">
+        <v>27</v>
+      </c>
+      <c r="J7" s="71">
+        <v>27</v>
+      </c>
+      <c r="K7" s="71">
+        <v>76.5</v>
+      </c>
+      <c r="L7" s="88">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="95">
+        <v>9</v>
+      </c>
+      <c r="D8" s="82">
+        <v>7.83</v>
+      </c>
+      <c r="E8" s="70">
+        <v>74.28</v>
+      </c>
+      <c r="F8" s="70">
+        <v>12.05</v>
+      </c>
+      <c r="G8" s="70">
+        <v>5.01</v>
+      </c>
+      <c r="H8" s="83">
+        <v>0.83</v>
+      </c>
+      <c r="I8" s="89">
+        <v>87.7</v>
+      </c>
+      <c r="J8" s="72">
+        <v>87.7</v>
+      </c>
+      <c r="K8" s="72">
+        <v>348.6</v>
+      </c>
+      <c r="L8" s="90">
+        <v>161.30000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="94" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="95">
+        <v>4</v>
+      </c>
+      <c r="D9" s="82">
+        <v>7.46</v>
+      </c>
+      <c r="E9" s="70">
+        <v>63.68</v>
+      </c>
+      <c r="F9" s="70">
+        <v>9.44</v>
+      </c>
+      <c r="G9" s="70">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="H9" s="83">
+        <v>9.64</v>
+      </c>
+      <c r="I9" s="87">
+        <v>3.5</v>
+      </c>
+      <c r="J9" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="K9" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="L9" s="88">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="94" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="95">
+        <v>3</v>
+      </c>
+      <c r="D10" s="82">
+        <v>9.08</v>
+      </c>
+      <c r="E10" s="70">
+        <v>63.32</v>
+      </c>
+      <c r="F10" s="70">
+        <v>15.25</v>
+      </c>
+      <c r="G10" s="70">
+        <v>11.5</v>
+      </c>
+      <c r="H10" s="83">
+        <v>0.85</v>
+      </c>
+      <c r="I10" s="87">
+        <v>9.1</v>
+      </c>
+      <c r="J10" s="71">
+        <v>9.1</v>
+      </c>
+      <c r="K10" s="71">
+        <v>29</v>
+      </c>
+      <c r="L10" s="88">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="95">
+        <v>3</v>
+      </c>
+      <c r="D11" s="82">
+        <v>6.68</v>
+      </c>
+      <c r="E11" s="70">
+        <v>71.17</v>
+      </c>
+      <c r="F11" s="70">
+        <v>9.23</v>
+      </c>
+      <c r="G11" s="70">
+        <v>10.01</v>
+      </c>
+      <c r="H11" s="83">
+        <v>2.91</v>
+      </c>
+      <c r="I11" s="87">
+        <v>3.9</v>
+      </c>
+      <c r="J11" s="71">
+        <v>3.9</v>
+      </c>
+      <c r="K11" s="71">
+        <v>3.9</v>
+      </c>
+      <c r="L11" s="88">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="95">
+        <v>3</v>
+      </c>
+      <c r="D12" s="82">
+        <v>7.12</v>
+      </c>
+      <c r="E12" s="70">
+        <v>68.53</v>
+      </c>
+      <c r="F12" s="70">
+        <v>11.11</v>
+      </c>
+      <c r="G12" s="70">
+        <v>12.11</v>
+      </c>
+      <c r="H12" s="83">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="I12" s="87">
         <v>5.9</v>
       </c>
-      <c r="L3" s="123">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="109" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="110">
+      <c r="J12" s="71">
+        <v>5.9</v>
+      </c>
+      <c r="K12" s="71">
+        <v>7.5</v>
+      </c>
+      <c r="L12" s="88">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="94" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="95">
+        <v>3</v>
+      </c>
+      <c r="D13" s="82">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="E13" s="70">
+        <v>60.25</v>
+      </c>
+      <c r="F13" s="70">
+        <v>11.81</v>
+      </c>
+      <c r="G13" s="70">
+        <v>17.260000000000002</v>
+      </c>
+      <c r="H13" s="83">
+        <v>1.3</v>
+      </c>
+      <c r="I13" s="87">
         <v>9</v>
       </c>
-      <c r="D4" s="92">
-        <v>9.61</v>
-      </c>
-      <c r="E4" s="72">
-        <v>63.86</v>
-      </c>
-      <c r="F4" s="72">
-        <v>12.76</v>
-      </c>
-      <c r="G4" s="72">
-        <v>13.01</v>
-      </c>
-      <c r="H4" s="93">
-        <v>0.75</v>
-      </c>
-      <c r="I4" s="97">
-        <v>27</v>
-      </c>
-      <c r="J4" s="73">
-        <v>27</v>
-      </c>
-      <c r="K4" s="73">
-        <v>78</v>
-      </c>
-      <c r="L4" s="98">
-        <v>48.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="111" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="110">
+      <c r="J13" s="71">
         <v>9</v>
       </c>
-      <c r="D5" s="92">
-        <v>4.41</v>
-      </c>
-      <c r="E5" s="72">
-        <v>45.24</v>
-      </c>
-      <c r="F5" s="72">
-        <v>23.74</v>
-      </c>
-      <c r="G5" s="72">
-        <v>25.3</v>
-      </c>
-      <c r="H5" s="93">
-        <v>1.31</v>
-      </c>
-      <c r="I5" s="97">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="J5" s="73">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="K5" s="73">
-        <v>5.5</v>
-      </c>
-      <c r="L5" s="98">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="109" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="110">
-        <v>9</v>
-      </c>
-      <c r="D6" s="92">
-        <v>7.52</v>
-      </c>
-      <c r="E6" s="72">
-        <v>69.650000000000006</v>
-      </c>
-      <c r="F6" s="72">
-        <v>10.69</v>
-      </c>
-      <c r="G6" s="72">
-        <v>11.27</v>
-      </c>
-      <c r="H6" s="93">
-        <v>0.87</v>
-      </c>
-      <c r="I6" s="97">
-        <v>15.6</v>
-      </c>
-      <c r="J6" s="73">
-        <v>15.6</v>
-      </c>
-      <c r="K6" s="73">
-        <v>35</v>
-      </c>
-      <c r="L6" s="98">
-        <v>26.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="109" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="110">
-        <v>9</v>
-      </c>
-      <c r="D7" s="92">
-        <v>10.84</v>
-      </c>
-      <c r="E7" s="72">
-        <v>66.67</v>
-      </c>
-      <c r="F7" s="72">
-        <v>9.57</v>
-      </c>
-      <c r="G7" s="72">
-        <v>12.12</v>
-      </c>
-      <c r="H7" s="93">
-        <v>0.8</v>
-      </c>
-      <c r="I7" s="97">
-        <v>27</v>
-      </c>
-      <c r="J7" s="73">
-        <v>27</v>
-      </c>
-      <c r="K7" s="73">
-        <v>76.5</v>
-      </c>
-      <c r="L7" s="98">
-        <v>48.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="109" t="s">
+      <c r="K13" s="71">
+        <v>28.1</v>
+      </c>
+      <c r="L13" s="88">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="110">
-        <v>9</v>
-      </c>
-      <c r="D8" s="92">
-        <v>7.83</v>
-      </c>
-      <c r="E8" s="72">
-        <v>74.28</v>
-      </c>
-      <c r="F8" s="72">
-        <v>12.05</v>
-      </c>
-      <c r="G8" s="72">
-        <v>5.01</v>
-      </c>
-      <c r="H8" s="93">
-        <v>0.83</v>
-      </c>
-      <c r="I8" s="99">
-        <v>87.7</v>
-      </c>
-      <c r="J8" s="74">
-        <v>87.7</v>
-      </c>
-      <c r="K8" s="74">
-        <v>348.6</v>
-      </c>
-      <c r="L8" s="100">
-        <v>161.30000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="109" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="71" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="110">
-        <v>4</v>
-      </c>
-      <c r="D9" s="92">
-        <v>7.46</v>
-      </c>
-      <c r="E9" s="72">
-        <v>63.68</v>
-      </c>
-      <c r="F9" s="72">
-        <v>9.44</v>
-      </c>
-      <c r="G9" s="72">
-        <v>9.7799999999999994</v>
-      </c>
-      <c r="H9" s="93">
-        <v>9.64</v>
-      </c>
-      <c r="I9" s="97">
-        <v>3.5</v>
-      </c>
-      <c r="J9" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="K9" s="73">
-        <v>3.5</v>
-      </c>
-      <c r="L9" s="98">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="109" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="71" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="110">
-        <v>3</v>
-      </c>
-      <c r="D10" s="92">
-        <v>9.08</v>
-      </c>
-      <c r="E10" s="72">
-        <v>63.32</v>
-      </c>
-      <c r="F10" s="72">
-        <v>15.25</v>
-      </c>
-      <c r="G10" s="72">
-        <v>11.5</v>
-      </c>
-      <c r="H10" s="93">
-        <v>0.85</v>
-      </c>
-      <c r="I10" s="97">
-        <v>9.1</v>
-      </c>
-      <c r="J10" s="73">
-        <v>9.1</v>
-      </c>
-      <c r="K10" s="73">
-        <v>29</v>
-      </c>
-      <c r="L10" s="98">
-        <v>16.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="109" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="71" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="110">
-        <v>3</v>
-      </c>
-      <c r="D11" s="92">
-        <v>6.68</v>
-      </c>
-      <c r="E11" s="72">
-        <v>71.17</v>
-      </c>
-      <c r="F11" s="72">
-        <v>9.23</v>
-      </c>
-      <c r="G11" s="72">
-        <v>10.01</v>
-      </c>
-      <c r="H11" s="93">
-        <v>2.91</v>
-      </c>
-      <c r="I11" s="97">
-        <v>3.9</v>
-      </c>
-      <c r="J11" s="73">
-        <v>3.9</v>
-      </c>
-      <c r="K11" s="73">
-        <v>3.9</v>
-      </c>
-      <c r="L11" s="98">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="109" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="71" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="110">
-        <v>3</v>
-      </c>
-      <c r="D12" s="92">
-        <v>7.12</v>
-      </c>
-      <c r="E12" s="72">
-        <v>68.53</v>
-      </c>
-      <c r="F12" s="72">
-        <v>11.11</v>
-      </c>
-      <c r="G12" s="72">
-        <v>12.11</v>
-      </c>
-      <c r="H12" s="93">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="I12" s="97">
-        <v>5.9</v>
-      </c>
-      <c r="J12" s="73">
-        <v>5.9</v>
-      </c>
-      <c r="K12" s="73">
-        <v>7.5</v>
-      </c>
-      <c r="L12" s="98">
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="109" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="71" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="110">
-        <v>3</v>
-      </c>
-      <c r="D13" s="92">
-        <v>9.3699999999999992</v>
-      </c>
-      <c r="E13" s="72">
-        <v>60.25</v>
-      </c>
-      <c r="F13" s="72">
-        <v>11.81</v>
-      </c>
-      <c r="G13" s="72">
-        <v>17.260000000000002</v>
-      </c>
-      <c r="H13" s="93">
-        <v>1.3</v>
-      </c>
-      <c r="I13" s="97">
-        <v>9</v>
-      </c>
-      <c r="J13" s="73">
-        <v>9</v>
-      </c>
-      <c r="K13" s="73">
-        <v>28.1</v>
-      </c>
-      <c r="L13" s="98">
-        <v>16.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="112" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="113" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="114">
-        <v>3</v>
-      </c>
-      <c r="D14" s="94">
+      <c r="B14" s="98" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="99">
+        <v>3</v>
+      </c>
+      <c r="D14" s="84">
         <v>7.51</v>
       </c>
-      <c r="E14" s="95">
+      <c r="E14" s="85">
         <v>72.959999999999994</v>
       </c>
-      <c r="F14" s="95">
+      <c r="F14" s="85">
         <v>12.65</v>
       </c>
-      <c r="G14" s="95">
+      <c r="G14" s="85">
         <v>5.98</v>
       </c>
-      <c r="H14" s="96">
+      <c r="H14" s="86">
         <v>0.9</v>
       </c>
-      <c r="I14" s="101">
+      <c r="I14" s="91">
         <v>31.2</v>
       </c>
-      <c r="J14" s="102">
+      <c r="J14" s="92">
         <v>31.2</v>
       </c>
-      <c r="K14" s="102">
+      <c r="K14" s="92">
         <v>115.2</v>
       </c>
-      <c r="L14" s="103">
+      <c r="L14" s="93">
         <v>60.5</v>
       </c>
     </row>
@@ -5292,20 +5289,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="87" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="88"/>
+      <c r="A1" s="132" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="130" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="131"/>
     </row>
     <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="34" t="s">
@@ -5355,10 +5352,10 @@
       <c r="E3" s="39">
         <v>100</v>
       </c>
-      <c r="F3" s="69">
+      <c r="F3" s="67">
         <v>0.23</v>
       </c>
-      <c r="G3" s="69">
+      <c r="G3" s="67">
         <f>H3+I3</f>
         <v>3653429.8499999996</v>
       </c>
@@ -5368,7 +5365,7 @@
       <c r="I3" s="48">
         <v>331.82</v>
       </c>
-      <c r="J3" s="75">
+      <c r="J3" s="73">
         <f>I3/E3</f>
         <v>3.3182</v>
       </c>
@@ -5389,21 +5386,15 @@
       <c r="E4" s="4">
         <v>100</v>
       </c>
-      <c r="F4" s="68">
+      <c r="F4" s="66">
         <v>0.34200000000000003</v>
       </c>
       <c r="G4" s="22">
         <v>68531.157000000007</v>
       </c>
-      <c r="H4" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H4" s="135"/>
+      <c r="I4" s="135"/>
+      <c r="J4" s="136"/>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
@@ -5492,7 +5483,7 @@
       <c r="F7" s="24">
         <v>0.11</v>
       </c>
-      <c r="G7" s="68">
+      <c r="G7" s="66">
         <f t="shared" si="0"/>
         <v>1974938.16</v>
       </c>
@@ -5502,7 +5493,7 @@
       <c r="I7" s="24">
         <v>333.96</v>
       </c>
-      <c r="J7" s="76">
+      <c r="J7" s="74">
         <f t="shared" si="1"/>
         <v>3.3395999999999999</v>
       </c>
@@ -5529,15 +5520,9 @@
       <c r="G8" s="22">
         <v>499202.08500000002</v>
       </c>
-      <c r="H8" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H8" s="135"/>
+      <c r="I8" s="135"/>
+      <c r="J8" s="136"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
@@ -5663,15 +5648,9 @@
       <c r="G12" s="22">
         <v>1085465.2709999999</v>
       </c>
-      <c r="H12" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H12" s="135"/>
+      <c r="I12" s="135"/>
+      <c r="J12" s="136"/>
     </row>
     <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
@@ -5797,15 +5776,9 @@
       <c r="G16" s="22">
         <v>2730211.4580000001</v>
       </c>
-      <c r="H16" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H16" s="135"/>
+      <c r="I16" s="135"/>
+      <c r="J16" s="136"/>
     </row>
     <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
@@ -5931,15 +5904,9 @@
       <c r="G20" s="22">
         <v>1074019.6839999999</v>
       </c>
-      <c r="H20" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I20" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H20" s="135"/>
+      <c r="I20" s="135"/>
+      <c r="J20" s="136"/>
     </row>
     <row r="21" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
@@ -6065,15 +6032,9 @@
       <c r="G24" s="22">
         <v>2676741.4920000001</v>
       </c>
-      <c r="H24" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H24" s="135"/>
+      <c r="I24" s="135"/>
+      <c r="J24" s="136"/>
     </row>
     <row r="25" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
@@ -6199,15 +6160,9 @@
       <c r="G28" s="22">
         <v>550808.13899999997</v>
       </c>
-      <c r="H28" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I28" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J28" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H28" s="135"/>
+      <c r="I28" s="135"/>
+      <c r="J28" s="136"/>
     </row>
     <row r="29" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="25" t="s">
@@ -6333,15 +6288,9 @@
       <c r="G32" s="22">
         <v>1363532.632</v>
       </c>
-      <c r="H32" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I32" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J32" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H32" s="135"/>
+      <c r="I32" s="135"/>
+      <c r="J32" s="136"/>
     </row>
     <row r="33" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
@@ -6467,15 +6416,9 @@
       <c r="G36" s="22">
         <v>149086.54199999999</v>
       </c>
-      <c r="H36" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I36" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J36" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H36" s="135"/>
+      <c r="I36" s="135"/>
+      <c r="J36" s="136"/>
     </row>
     <row r="37" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
@@ -6601,15 +6544,9 @@
       <c r="G40" s="22">
         <v>358690.42099999997</v>
       </c>
-      <c r="H40" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I40" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J40" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H40" s="135"/>
+      <c r="I40" s="135"/>
+      <c r="J40" s="136"/>
     </row>
     <row r="41" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="25" t="s">
@@ -6698,7 +6635,7 @@
       <c r="F43" s="48">
         <v>2.3864999999999998</v>
       </c>
-      <c r="G43" s="69">
+      <c r="G43" s="67">
         <f t="shared" si="0"/>
         <v>50936307.321000002</v>
       </c>
@@ -6732,18 +6669,12 @@
       <c r="F44" s="24">
         <v>2.9540000000000002</v>
       </c>
-      <c r="G44" s="68">
+      <c r="G44" s="66">
         <v>4503845.3099999996</v>
       </c>
-      <c r="H44" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I44" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J44" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H44" s="135"/>
+      <c r="I44" s="135"/>
+      <c r="J44" s="136"/>
     </row>
     <row r="45" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
@@ -6764,7 +6695,7 @@
       <c r="F45" s="24">
         <v>3.1869999999999998</v>
       </c>
-      <c r="G45" s="68">
+      <c r="G45" s="66">
         <f t="shared" si="0"/>
         <v>5288750.9240000006</v>
       </c>
@@ -6798,7 +6729,7 @@
       <c r="F46" s="24">
         <v>4.3319999999999999</v>
       </c>
-      <c r="G46" s="68">
+      <c r="G46" s="66">
         <f t="shared" si="0"/>
         <v>2903779.5300000003</v>
       </c>
@@ -6832,7 +6763,7 @@
       <c r="F47" s="24">
         <v>1.17</v>
       </c>
-      <c r="G47" s="68">
+      <c r="G47" s="66">
         <f t="shared" si="0"/>
         <v>44278301.408999994</v>
       </c>
@@ -6866,18 +6797,12 @@
       <c r="F48" s="24">
         <v>4.1595000000000004</v>
       </c>
-      <c r="G48" s="68">
+      <c r="G48" s="66">
         <v>11383143.26</v>
       </c>
-      <c r="H48" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="I48" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="J48" s="54" t="s">
-        <v>34</v>
-      </c>
+      <c r="H48" s="135"/>
+      <c r="I48" s="135"/>
+      <c r="J48" s="136"/>
     </row>
     <row r="49" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="25" t="s">
@@ -6895,10 +6820,10 @@
       <c r="E49" s="21">
         <v>22000</v>
       </c>
-      <c r="F49" s="81">
+      <c r="F49" s="79">
         <v>0.93</v>
       </c>
-      <c r="G49" s="68">
+      <c r="G49" s="66">
         <f t="shared" si="0"/>
         <v>15206140.234999999</v>
       </c>
@@ -6932,7 +6857,7 @@
       <c r="F50" s="30">
         <v>1.296</v>
       </c>
-      <c r="G50" s="77">
+      <c r="G50" s="75">
         <f t="shared" si="0"/>
         <v>3898543.9180000001</v>
       </c>
@@ -6971,24 +6896,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="78" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="80" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="81" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1">
@@ -6999,10 +6924,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="81" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1">
@@ -7013,10 +6938,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="81" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1">
@@ -7027,10 +6952,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="81" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1">
@@ -7041,10 +6966,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="81" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1">
@@ -7055,10 +6980,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="81" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1">
@@ -7069,10 +6994,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="81" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1">
@@ -7083,10 +7008,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="81" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="1">
@@ -7097,10 +7022,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="81" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1">
@@ -7111,10 +7036,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="81" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1">
@@ -7125,10 +7050,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="81" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1">
@@ -7139,10 +7064,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="81" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1">

</xml_diff>